<commit_message>
performance comparison with other similar projects
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -209,6 +209,48 @@
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="2.7777777777777693E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="1.8518518518518517E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -305,7 +347,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0" formatCode="0%">
-                  <c:v>0.72</c:v>
+                  <c:v>0.73</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.76600000000000001</c:v>
@@ -328,11 +370,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="199255552"/>
-        <c:axId val="199255944"/>
+        <c:axId val="203678200"/>
+        <c:axId val="203680632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="199255552"/>
+        <c:axId val="203678200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -375,7 +417,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199255944"/>
+        <c:crossAx val="203680632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -383,7 +425,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199255944"/>
+        <c:axId val="203680632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -434,7 +476,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199255552"/>
+        <c:crossAx val="203678200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1351,7 +1393,7 @@
   <dimension ref="C5:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="2">
-        <v>0.72</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>